<commit_message>
feat: contamination, spearman's tests PCBi + synthesis trends + maps ROCCHMV
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/PCBi/summarised_levels_data_PCBi_lw.xlsx
+++ b/inst/results/data_contam/PCBi/summarised_levels_data_PCBi_lw.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,175 +361,270 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ESTUARY</t>
+          <t>PARAMETRE_LIBELLE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>PARAMETRE_LIBELLE</t>
+          <t>First 5 years</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>median_ng_glw</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>median_1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median_2</t>
+          <t>Last 5 years</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>CB 101</t>
         </is>
       </c>
+      <c r="B2">
+        <v>272.0365</v>
+      </c>
       <c r="C2">
-        <v>77.557</v>
-      </c>
-      <c r="D2">
-        <v>129.9</v>
-      </c>
-      <c r="E2">
-        <v>64.09999999999999</v>
+        <v>70.39949999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Loire</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CB 101</t>
-        </is>
+          <t>CB 118</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>172.653</v>
       </c>
       <c r="C3">
-        <v>58.76000000000001</v>
-      </c>
-      <c r="D3">
-        <v>203.1</v>
-      </c>
-      <c r="E3">
-        <v>48.56</v>
+        <v>40.273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Seine</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CB 101</t>
-        </is>
+          <t>CB 138</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>892.4010000000001</v>
       </c>
       <c r="C4">
-        <v>569.072</v>
-      </c>
-      <c r="D4">
-        <v>1492</v>
-      </c>
-      <c r="E4">
-        <v>470.3</v>
+        <v>147.5985</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CB 118</t>
-        </is>
+          <t>CB 153</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>1391.7845</v>
       </c>
       <c r="C5">
-        <v>37.815</v>
-      </c>
-      <c r="D5">
-        <v>235.2</v>
-      </c>
-      <c r="E5">
-        <v>151.3</v>
+        <v>473.5635</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Loire</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CB 118</t>
-        </is>
+          <t>CB 180</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>202.905</v>
       </c>
       <c r="C6">
-        <v>38.126</v>
-      </c>
-      <c r="D6">
-        <v>632.4</v>
-      </c>
-      <c r="E6">
-        <v>152.5</v>
+        <v>46.172</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Seine</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CB 118</t>
-        </is>
+          <t>CB 28</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>13.495</v>
       </c>
       <c r="C7">
-        <v>373.984</v>
-      </c>
-      <c r="D7">
-        <v>6134</v>
-      </c>
-      <c r="E7">
-        <v>1496</v>
+        <v>1.9855</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>CB 52</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>65.95699999999999</v>
+      </c>
+      <c r="C8">
+        <v>14.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTUARY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PARAMETRE_LIBELLE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>First 5 years</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last 5 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>Gironde</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CB 101</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>157.119</v>
+      </c>
+      <c r="D2">
+        <v>77.557</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CB 101</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>245.7235</v>
+      </c>
+      <c r="D3">
+        <v>58.76000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CB 101</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>1805.3425</v>
+      </c>
+      <c r="D4">
+        <v>569.072</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CB 118</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>58.799</v>
+      </c>
+      <c r="D5">
+        <v>37.815</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CB 118</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>158.1035</v>
+      </c>
+      <c r="D6">
+        <v>38.126</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CB 118</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>1533.4485</v>
+      </c>
+      <c r="D7">
+        <v>373.984</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>CB 138</t>
         </is>
       </c>
       <c r="C8">
+        <v>527.2635</v>
+      </c>
+      <c r="D8">
         <v>128.1725</v>
-      </c>
-      <c r="D8">
-        <v>166.3</v>
-      </c>
-      <c r="E8">
-        <v>40.43</v>
       </c>
     </row>
     <row r="9">
@@ -543,13 +639,10 @@
         </is>
       </c>
       <c r="C9">
+        <v>839.3395</v>
+      </c>
+      <c r="D9">
         <v>122.254</v>
-      </c>
-      <c r="D9">
-        <v>264.8</v>
-      </c>
-      <c r="E9">
-        <v>38.57</v>
       </c>
     </row>
     <row r="10">
@@ -564,13 +657,10 @@
         </is>
       </c>
       <c r="C10">
+        <v>2982.968</v>
+      </c>
+      <c r="D10">
         <v>875.9014999999999</v>
-      </c>
-      <c r="D10">
-        <v>941</v>
-      </c>
-      <c r="E10">
-        <v>276.3</v>
       </c>
     </row>
     <row r="11">
@@ -585,13 +675,10 @@
         </is>
       </c>
       <c r="C11">
+        <v>1122.002</v>
+      </c>
+      <c r="D11">
         <v>603.847</v>
-      </c>
-      <c r="D11">
-        <v>70.79000000000001</v>
-      </c>
-      <c r="E11">
-        <v>38.1</v>
       </c>
     </row>
     <row r="12">
@@ -606,13 +693,10 @@
         </is>
       </c>
       <c r="C12">
+        <v>1126.1245</v>
+      </c>
+      <c r="D12">
         <v>310.6785</v>
-      </c>
-      <c r="D12">
-        <v>71.05</v>
-      </c>
-      <c r="E12">
-        <v>19.6</v>
       </c>
     </row>
     <row r="13">
@@ -627,13 +711,10 @@
         </is>
       </c>
       <c r="C13">
+        <v>3999.73</v>
+      </c>
+      <c r="D13">
         <v>1530.8605</v>
-      </c>
-      <c r="D13">
-        <v>252.3</v>
-      </c>
-      <c r="E13">
-        <v>96.58</v>
       </c>
     </row>
     <row r="14">
@@ -648,13 +729,10 @@
         </is>
       </c>
       <c r="C14">
+        <v>202.905</v>
+      </c>
+      <c r="D14">
         <v>67.52250000000001</v>
-      </c>
-      <c r="D14">
-        <v>43.26</v>
-      </c>
-      <c r="E14">
-        <v>14.4</v>
       </c>
     </row>
     <row r="15">
@@ -669,13 +747,10 @@
         </is>
       </c>
       <c r="C15">
+        <v>107.019</v>
+      </c>
+      <c r="D15">
         <v>22.0375</v>
-      </c>
-      <c r="D15">
-        <v>22.82</v>
-      </c>
-      <c r="E15">
-        <v>4.699</v>
       </c>
     </row>
     <row r="16">
@@ -690,13 +765,10 @@
         </is>
       </c>
       <c r="C16">
+        <v>369.52</v>
+      </c>
+      <c r="D16">
         <v>97.8295</v>
-      </c>
-      <c r="D16">
-        <v>78.79000000000001</v>
-      </c>
-      <c r="E16">
-        <v>20.86</v>
       </c>
     </row>
     <row r="17">
@@ -711,13 +783,10 @@
         </is>
       </c>
       <c r="C17">
+        <v>12.531</v>
+      </c>
+      <c r="D17">
         <v>1.995</v>
-      </c>
-      <c r="D17">
-        <v>18.7</v>
-      </c>
-      <c r="E17">
-        <v>2.978</v>
       </c>
     </row>
     <row r="18">
@@ -732,13 +801,10 @@
         </is>
       </c>
       <c r="C18">
+        <v>6.466</v>
+      </c>
+      <c r="D18">
         <v>1.6035</v>
-      </c>
-      <c r="D18">
-        <v>9.651</v>
-      </c>
-      <c r="E18">
-        <v>2.393</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +819,10 @@
         </is>
       </c>
       <c r="C19">
+        <v>62.947</v>
+      </c>
+      <c r="D19">
         <v>12.094</v>
-      </c>
-      <c r="D19">
-        <v>93.95</v>
-      </c>
-      <c r="E19">
-        <v>18.05</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +837,10 @@
         </is>
       </c>
       <c r="C20">
+        <v>51.0875</v>
+      </c>
+      <c r="D20">
         <v>19.163</v>
-      </c>
-      <c r="D20">
-        <v>47.3</v>
-      </c>
-      <c r="E20">
-        <v>17.74</v>
       </c>
     </row>
     <row r="21">
@@ -795,13 +855,10 @@
         </is>
       </c>
       <c r="C21">
+        <v>47.8515</v>
+      </c>
+      <c r="D21">
         <v>11.8725</v>
-      </c>
-      <c r="D21">
-        <v>44.31</v>
-      </c>
-      <c r="E21">
-        <v>10.99</v>
       </c>
     </row>
     <row r="22">
@@ -816,13 +873,10 @@
         </is>
       </c>
       <c r="C22">
+        <v>542.3315</v>
+      </c>
+      <c r="D22">
         <v>136.279</v>
-      </c>
-      <c r="D22">
-        <v>502.2</v>
-      </c>
-      <c r="E22">
-        <v>126.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>